<commit_message>
10/21/16 some aliases and shell func work
</commit_message>
<xml_diff>
--- a/svbWebPaymentUsers/MarkFinalQA.xlsx
+++ b/svbWebPaymentUsers/MarkFinalQA.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="1180" windowWidth="20460" windowHeight="17600" tabRatio="332" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="3320" yWindow="20" windowWidth="20460" windowHeight="17600" tabRatio="332" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mark QA" sheetId="1" r:id="rId1"/>
     <sheet name="master" sheetId="2" r:id="rId2"/>
     <sheet name="ReArranged" sheetId="3" r:id="rId3"/>
     <sheet name="AcctNumSort" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Sort by name then acct" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -879,125 +879,7 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF000090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9411A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD81C20"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF11E634"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="45">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4269,42 +4151,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N26:N28 M29:M1048576 M1:M25">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>20105134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>20103239</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
       <formula>20102682</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>20102674</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>20102666</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>20102631</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>20102623</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>20102615</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>20133790</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
       <formula>20100175</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
       <formula>20100167</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>20100175</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4322,7 +4204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -5773,37 +5655,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E25:E27">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>20105134</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>20103239</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>20102682</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>20102674</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>20102666</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>20102631</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>20102623</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>20102615</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>20133790</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>20100175</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>20100167</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7270,1450 +7152,6 @@
     <sortCondition ref="D2:D27"/>
   </sortState>
   <conditionalFormatting sqref="E25:E27">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
-      <formula>20105134</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
-      <formula>20103239</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
-      <formula>20102682</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
-      <formula>20102674</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
-      <formula>20102666</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
-      <formula>20102631</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
-      <formula>20102623</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
-      <formula>20102615</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
-      <formula>20133790</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
-      <formula>20100175</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
-      <formula>20100167</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:45" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A2" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1496806</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E2" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="2">
-        <v>200</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>500</v>
-      </c>
-      <c r="J2" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="AF2" s="4">
-        <v>5167510</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>1472708</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A3" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1496806</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="2">
-        <v>200</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I3" s="2">
-        <v>500</v>
-      </c>
-      <c r="J3" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A4" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1496806</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E4" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="2">
-        <v>200</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I4" s="2">
-        <v>500</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A5" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1142212</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="11">
-        <v>20100167</v>
-      </c>
-      <c r="E5" s="11">
-        <v>2102897</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="2">
-        <v>200</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I5" s="2">
-        <v>500</v>
-      </c>
-      <c r="J5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A6" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1142212</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="11">
-        <v>20100175</v>
-      </c>
-      <c r="E6" s="11">
-        <v>2102896</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="2">
-        <v>200</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I6" s="2">
-        <v>500</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A7" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1142212</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="11">
-        <v>20133790</v>
-      </c>
-      <c r="E7" s="11">
-        <v>81325842</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="2">
-        <v>200</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I7" s="2">
-        <v>500</v>
-      </c>
-      <c r="J7" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A8" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1496805</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="2">
-        <v>200</v>
-      </c>
-      <c r="H8" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I8" s="2">
-        <v>500</v>
-      </c>
-      <c r="J8" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A9" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1496805</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E9" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="2">
-        <v>200</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>500</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A10" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1496805</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E10" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="2">
-        <v>200</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I10" s="2">
-        <v>500</v>
-      </c>
-      <c r="J10" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U10" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A11" s="6">
-        <v>5167510</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1472708</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="2">
-        <v>20127596</v>
-      </c>
-      <c r="E11" s="2">
-        <v>53597706</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="2">
-        <v>200</v>
-      </c>
-      <c r="H11" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I11" s="2">
-        <v>500</v>
-      </c>
-      <c r="J11" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U11" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A12" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1101463</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E12" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="2">
-        <v>200</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I12" s="2">
-        <v>500</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A13" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1101463</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E13" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="2">
-        <v>200</v>
-      </c>
-      <c r="H13" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I13" s="2">
-        <v>500</v>
-      </c>
-      <c r="J13" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U13" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A14" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1101463</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E14" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="2">
-        <v>200</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I14" s="2">
-        <v>500</v>
-      </c>
-      <c r="J14" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U14" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A15" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1142226</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E15" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="2">
-        <v>200</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I15" s="2">
-        <v>500</v>
-      </c>
-      <c r="J15" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U15" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" s="2" customFormat="1" ht="20">
-      <c r="A16" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1142226</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E16" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="2">
-        <v>200</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I16" s="2">
-        <v>500</v>
-      </c>
-      <c r="J16" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A17" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1142226</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E17" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="2">
-        <v>200</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I17" s="2">
-        <v>500</v>
-      </c>
-      <c r="J17" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U17" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A18" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B18" s="13">
-        <v>1100798</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E18" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="2">
-        <v>200</v>
-      </c>
-      <c r="H18" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I18" s="2">
-        <v>500</v>
-      </c>
-      <c r="J18" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U18" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A19" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B19" s="13">
-        <v>1100798</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E19" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="2">
-        <v>200</v>
-      </c>
-      <c r="H19" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I19" s="2">
-        <v>500</v>
-      </c>
-      <c r="J19" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A20" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B20" s="13">
-        <v>1100798</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E20" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="2">
-        <v>200</v>
-      </c>
-      <c r="H20" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I20" s="2">
-        <v>500</v>
-      </c>
-      <c r="J20" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U20" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A21" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1101460</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="5">
-        <v>20100167</v>
-      </c>
-      <c r="E21" s="5">
-        <v>2102897</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="2">
-        <v>200</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I21" s="2">
-        <v>500</v>
-      </c>
-      <c r="J21" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U21" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A22" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1101460</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="5">
-        <v>20100175</v>
-      </c>
-      <c r="E22" s="5">
-        <v>2102896</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="2">
-        <v>200</v>
-      </c>
-      <c r="H22" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I22" s="2">
-        <v>500</v>
-      </c>
-      <c r="J22" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U22" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A23" s="6">
-        <v>5030870</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1101460</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="5">
-        <v>20133790</v>
-      </c>
-      <c r="E23" s="5">
-        <v>81325842</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="2">
-        <v>200</v>
-      </c>
-      <c r="H23" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I23" s="2">
-        <v>500</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U23" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A24" s="6">
-        <v>5167510</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1473036</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="5">
-        <v>20127596</v>
-      </c>
-      <c r="E24" s="5">
-        <v>53597706</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="2">
-        <v>200</v>
-      </c>
-      <c r="H24" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I24" s="2">
-        <v>500</v>
-      </c>
-      <c r="J24" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U24" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A25" s="6">
-        <v>5107936</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1276339</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="2">
-        <v>20104448</v>
-      </c>
-      <c r="E25" s="2">
-        <v>6665576</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" s="2">
-        <v>200</v>
-      </c>
-      <c r="H25" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I25" s="2">
-        <v>500</v>
-      </c>
-      <c r="J25" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U25" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A26" s="6">
-        <v>5107936</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1276339</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="2">
-        <v>20104472</v>
-      </c>
-      <c r="E26" s="2">
-        <v>6665767</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="2">
-        <v>200</v>
-      </c>
-      <c r="H26" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I26" s="2">
-        <v>500</v>
-      </c>
-      <c r="J26" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U26" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" s="2" customFormat="1" ht="20">
-      <c r="A27" s="6">
-        <v>5107936</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1276339</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="2">
-        <v>20125054</v>
-      </c>
-      <c r="E27" s="2">
-        <v>47820939</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="2">
-        <v>200</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2000</v>
-      </c>
-      <c r="I27" s="2">
-        <v>500</v>
-      </c>
-      <c r="J27" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U27" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:N27">
-    <sortCondition ref="C2:C27"/>
-    <sortCondition ref="D2:D27"/>
-  </sortState>
-  <conditionalFormatting sqref="E25:E27">
     <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>20105134</formula>
     </cfRule>
@@ -8749,6 +7187,1450 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:45" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A2" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1496806</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="2">
+        <v>200</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I2" s="2">
+        <v>500</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="AF2" s="4">
+        <v>5167510</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>1472708</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A3" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1496806</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2">
+        <v>200</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>500</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A4" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1496806</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E4" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2">
+        <v>200</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>500</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A5" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1142212</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="11">
+        <v>20100167</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2102897</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="2">
+        <v>200</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="2">
+        <v>500</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A6" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1142212</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="11">
+        <v>20100175</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2102896</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="2">
+        <v>200</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="2">
+        <v>500</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A7" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1142212</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="11">
+        <v>20133790</v>
+      </c>
+      <c r="E7" s="11">
+        <v>81325842</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="2">
+        <v>200</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I7" s="2">
+        <v>500</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A8" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1496805</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="2">
+        <v>200</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>500</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A9" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1496805</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="2">
+        <v>200</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I9" s="2">
+        <v>500</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A10" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1496805</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E10" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="2">
+        <v>200</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>500</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A11" s="6">
+        <v>5167510</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1472708</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="2">
+        <v>20127596</v>
+      </c>
+      <c r="E11" s="2">
+        <v>53597706</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2">
+        <v>200</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>500</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A12" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1101463</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="2">
+        <v>200</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I12" s="2">
+        <v>500</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A13" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1101463</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="2">
+        <v>200</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I13" s="2">
+        <v>500</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A14" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1101463</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E14" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="2">
+        <v>200</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="2">
+        <v>500</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A15" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1142226</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="2">
+        <v>200</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I15" s="2">
+        <v>500</v>
+      </c>
+      <c r="J15" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" s="2" customFormat="1" ht="20">
+      <c r="A16" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1142226</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="2">
+        <v>200</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="2">
+        <v>500</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A17" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1142226</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E17" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="2">
+        <v>200</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I17" s="2">
+        <v>500</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U17" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A18" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1100798</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="2">
+        <v>200</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I18" s="2">
+        <v>500</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A19" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1100798</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="2">
+        <v>200</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I19" s="2">
+        <v>500</v>
+      </c>
+      <c r="J19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A20" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1100798</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E20" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="2">
+        <v>200</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I20" s="2">
+        <v>500</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U20" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A21" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1101460</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5">
+        <v>20100167</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2102897</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="2">
+        <v>200</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I21" s="2">
+        <v>500</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A22" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1101460</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="5">
+        <v>20100175</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2102896</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="2">
+        <v>200</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="2">
+        <v>500</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A23" s="6">
+        <v>5030870</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1101460</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="5">
+        <v>20133790</v>
+      </c>
+      <c r="E23" s="5">
+        <v>81325842</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="2">
+        <v>200</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I23" s="2">
+        <v>500</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U23" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A24" s="6">
+        <v>5167510</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1473036</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="5">
+        <v>20127596</v>
+      </c>
+      <c r="E24" s="5">
+        <v>53597706</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="2">
+        <v>200</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I24" s="2">
+        <v>500</v>
+      </c>
+      <c r="J24" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A25" s="6">
+        <v>5107936</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1276339</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20104448</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6665576</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="2">
+        <v>200</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I25" s="2">
+        <v>500</v>
+      </c>
+      <c r="J25" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A26" s="6">
+        <v>5107936</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1276339</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2">
+        <v>20104472</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6665767</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="2">
+        <v>200</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I26" s="2">
+        <v>500</v>
+      </c>
+      <c r="J26" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U26" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="2" customFormat="1" ht="20">
+      <c r="A27" s="6">
+        <v>5107936</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1276339</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20125054</v>
+      </c>
+      <c r="E27" s="2">
+        <v>47820939</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="2">
+        <v>200</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I27" s="2">
+        <v>500</v>
+      </c>
+      <c r="J27" s="2">
+        <v>5000</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U27" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:N27">
+    <sortCondition ref="C2:C27"/>
+    <sortCondition ref="D2:D27"/>
+  </sortState>
+  <conditionalFormatting sqref="E25:E27">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>20105134</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>20103239</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>20102682</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>20102674</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>20102666</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>20102631</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>20102623</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>20102615</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+      <formula>20133790</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+      <formula>20100175</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+      <formula>20100167</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>